<commit_message>
pending, killcoda revisit, killersh
</commit_message>
<xml_diff>
--- a/cks_kcsa_kcna.xlsx
+++ b/cks_kcsa_kcna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiwen/Documents/wysi/project-cyber-monday/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29711623-AEF8-594F-8EFD-80CE2AB52710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BDED46-3018-F145-B1CF-14F7C142A311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17080" yWindow="220" windowWidth="17080" windowHeight="17800" activeTab="3" xr2:uid="{87DCA1D7-EB5D-4C4C-A7D2-7199B399E110}"/>
+    <workbookView xWindow="-18600" yWindow="-1460" windowWidth="18600" windowHeight="20020" xr2:uid="{87DCA1D7-EB5D-4C4C-A7D2-7199B399E110}"/>
   </bookViews>
   <sheets>
     <sheet name="kk_CKS" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="181">
   <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -564,12 +564,1237 @@
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Exam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AppArmor profile
+principle of least privilege
+serviceAccount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Secret
+base64 -d
+distribute credentials securely</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>manual static analysis
+security issues in config files</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># do not copy secret token, use and deletion in Dockerfile, as it's still stored in a few persistent layers even if we delete it afterwards.
+# do not expose plain text password value directly in env section of a pod, utilize k8s's secrets to store passwords
+# -e argument for turning escape sequence like `\n` into newline character
+echo -e "q3_file1.Dockerfile\nq3_file2.yaml" &gt; /opt/course/security-issues.txt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">k -n orion get po -oyaml | grep secret
+echo &lt;copy-and-paste-the-base64-encrypted-secret-here&gt; | base64 -d
+echo &lt;copy-and-paste-the-decoded-secret&gt; &gt; /root/CKS/secrets/CONNECTOR_PASSWORD
+# mount secret as volumes
+spec:
+  containers:
+    - name: test-container
+      volumeMounts:
+        - name: secret-volume
+          mountPath: /mnt/connector/password
+          readOnly: true
+  volumes:
+    - name: secret-volume
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>secret:
+        secretName:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> test-secret</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># move the json seccomp profile to /var/lib/kubelet/seccomp/profiles on the cp node
+mv /root/CKS/audit.json /var/lib/kubelet/seccomp/profiles
+# add spec.securityContext.seccompProfile.localhostProfile
+spec:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">  securityContext:
+    seccompProfile:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">      type: Localhost
+      localhostProfile: profiles/audit.json</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>json Seccomp profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># load AppArmor at controlplane
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>apparmor_parser</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> -q /etc/apparmor.d/frontend
+# verify the profile was successfully loaded
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>aa-status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> | grep restricted-frontend
+# you should be able to get result string `restricted-frontend` which is the profile name used by this file
+# edit pod spec.securityContext
+spec:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">  securityContext:
+    appArmorProfile:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">      type: Localhost
+      localhostProfile: restricted-frontend
+  serviceAccountName: frontend-default</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CIS benchmark report
+profile=false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi /etc/kubernetes/manifests/kube-controller-manager.yaml
+vi /etc/kubernetes/manifests/kube-scheduler.yaml
+# add command parameter --profiling=false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Falco
+change log output
+write log alerts
+falco_rules.local.yaml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPDX-Json SBOM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># install bom
+git clone https://github.com/kubernetes-sigs/bom.git
+cd bom
+go build -o bom ./cmd/bom
+mv bom /usr/local/bin/
+# generate sbom and save it to the desired file
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>bom generate --image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> registry.k8s.io/kube-apiserver:v1.31.0 \
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">  --format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> json \
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> --output </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>/opt/course/sbom1.json</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Admission Webhook Server
+AdmissionConfiguration
+admission-control-config-file
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># create admissionConfiguration file in the cp node
+# the /root/CKS/ImagePolicy/ on cp node is mounted to the /etc/admission-controllers/ directory in kube-apiserver
+cat &lt;&lt;EOF&gt; /root/CKS/ImagePolicy/admission-configuration.yaml
+apiVersion: apiserver.config.k8s.io/v1
+kind: AdmissionConfiguration
+plugins:
+- name: ImagePolicyWebhook
+  configuration:
+    imagePolicy:
+      kubeConfigFile: /etc/admission-controllers/admission-kubeconfig.yaml  # credentials to connect to webhook server
+      allowTTL: 50
+      denyTTL: 50
+      retryBackoff: 500
+      defaultAllow: false
+# update the kube-apiserver command flags and add ImagePolicyWebhook to enable admission plugins
+spec:
+  commands:
+    ...
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>- --admission-control-config-file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">=/etc/admission-controllers/admission-configuration.yaml
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> - --enable-admission-plugins</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>=NodeRestriction,ImagePolicyWebhook
+# in case of messing up, copy backup file back to the manifest directory
+cp -v /root/backup/kube-apiserver.yaml /etc/kubernetes/manifests</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NetworkPolicy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">k -n prod-x12cs get po,svc,netpol -owide --show-labels
+# checkout pod/redis-backend, service port number
+k -n prod-x12cs get netpol allow-redis-access -oyaml &gt; 2-1.yaml
+vi 2-1.yaml
+apiVersion: networking.k8s.io/v1
+kind: NetworkPolicy
+metadata:
+  name: allow-redis-access
+  namespace: prod-x12cs
+spec:
+  podSelector:
+    matchLabels:
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">run: redis-backend
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">  policyTypes:
+  - Ingress
+  ingress:
+  - from:
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>- namespaceSelector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">:
+        matchLabels:
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">access: redis
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>- podSelector:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+        matchLabels:
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>backend: prod-x12cs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+    ports:
+    - protocol: TCP
+      port: 6379
+k replace --force -f 2-1.yaml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">k -n team-azure get ciliumnetworkpolicy
+cat &lt;&lt;EOF&gt; deny-policy-p1.yaml
+apiVersion: "cilium.io/v2"
+kind: CiliumNetworkPolicy
+metadata:
+  name: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>p1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+  namespace: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>team-azure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+spec:
+  endpointSelector:
+    matchLabels:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">      role: messenger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+  egressDeny:
+  - toEndpoints:
+    - matchLabels:
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">  role: database</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+EOF
+k create -f deny-policy-p1.yaml
+# LAYER 3: 
+# communication between IP address (which source IP can send data to which destination IP)
+# the `endpointSelector` and `toEndpoints` define which pods (of certain IP address) can communicates with each other</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CiliumNetworkPolicy
+Layer 3 policy
+endpointSelector
+egressDeny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pod 
+  spec
+    automountServiceAccountToken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k -n gamma edit po apps-cluster-dash
+# add field spec.automountServiceAccountToken and set to false
+# remove the serviceAccountToken field</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Falco rules</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vi /etc/falco/falco_rules.local.yaml
+# find this rule
+/rule:.*shell 
+/desc:.*terminal
+/proc.tty
+# spawned_process and container         # a process inside a container
+# and shell_procs and proc.tty != 0     # a shell process w/ a terminal attached
+# and container_entrypoint ...
+# change output and priority
+  output: &gt;
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>%evt.time.s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>%user.uid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>%container.id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>%container.image.repository</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+  priority: ALERT
+# restart the falco service
+systemctl restart falco</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role
+user
+rolebinding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k -n dev-z edit role dev-user-access
+# change the rule to grant only get/list-pods access
+rules:
+  - apiGroups:
+    - ""
+    resources:
+    - pods
+    verbs:
+    - get
+    - list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pod security admission
+pod security standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k label ns team-red pod-security.kubernetes.io/enforce=baseline
+k -n team-red get po,rs,deploy
+k -n team-red delete po &lt;name-of-this-pod&gt;
+k -n team-red describe rs &lt;name-of-this-replicaset&gt;
+# copy the event error message, something about pod forbidden to create due to PodSecurity violation
+echo 'Warning  FailedCreate      5m17s (x9 over 16m)  replicaset-controller  (combined from similar events): Error creating: pods "hacker-f74b9f47d-jk9fn" is forbidden: violates PodSecurity "baseline:latest": hostPath volumes (volume "containerd-volume")' &gt; /opt/course/logs.txt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dockfile
+no curl
+version constraint
+no running process as root</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kubesec scan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kubesec scan /root/CKS/simple-pod.yaml
+# Remove the capabilities.add: SYS_ADMIN
+kubesec scan /root/CKS/simple-pod.yaml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audit Policy
+audit-policy-file
+audit-log-path
+audit-log-maxage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kube-bench report
+worker node authz mode
+protectKernelDefaults</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># need to protect node kernel parameter settings, make them non-overwritable by container workloads
+vi /var/lib/kubelet/config.yaml
+authorization:
+  mode: RBAC   # formerly alwaysAllow
+protectKernelDefaults: true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audit Policy
+audit-policy-file
+audit-log-path
+audit-log-maxage"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the same as task 2-9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cat &lt;&lt;EOF&gt; /etc/kubernetes/prod-audit.yaml
+apiVersion: audit.k8s.io/v1
+kind: Policy
+rules:
+- level: Metadata
+  verbs: delete
+  resources:
+  - group: ""
+    resources: ["secrets"]
+  namespaces: ["prod"]
+EOF
+vi /etc/kubernetes/manifests/kube-apiserver.yaml
+# add command flags
+  - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>--audit-policy-file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">=/etc/kubernetes/prod-audit.yaml
+  - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>--audit-log-path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">=/var/log/prod-secrets.log
+  - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>--audit-log-maxage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>=30
+# add volumes
+  - name: audit
+    hostPath:
+      path: /etc/kubernetes/prod-audit.yaml
+      type: File
+  - name: audit-log
+    hostPath:
+      path: /var/log/prod-secrets.log
+      type: FileOrCreate
+# add volumeMounts
+  - name: audit
+    mountPath: /etc/kubernetes/prod-audit.yaml
+    readOnly: true
+  - name: audit-log
+    mountPath: /var/log/prod-secrets.log
+    readOnly: false
+# esc and save, make sure the kube-apiserver restarts
+watch crictl ps</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kubesec scan /root/kubesec-pod.yaml
+# set containers[*].securityContext.privileged to false
+kubesec scan /root/kubesec-pod.yaml &gt; /root/kubesec_success_report.json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cp node kubeadm kubelet update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ssh cluster2-controlplane
+# edit the Kubernetes apt repository
+vi /etc/apt/sources.list.d/kubernetes.list
+deb [signed-by=/etc/apt/keyrings/kubernetes-apt-keyring.gpg] https://pkgs.k8s.io/core:/stable:/v1.31/deb/ /
+# to download k8s GPG public key, save it as binary in the directory `/etc/apt/keyrings/`
+echo 'y' | curl -fsSL https://pkgs.k8s.io/core:/stable:/v1.30/deb/Release.key | sudo gpg --yes --dearmor -o /etc/apt/keyrings/kubernetes-apt-keyring.gpg
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"># TODO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">verify that I can replace above commands with steps in below URL
+#      https://kubernetes.io/docs/setup/production-environment/tools/kubeadm/install-kubeadm/
+apt-get update
+apt-cache madison kubeadm
+apt-get install kubeadm=1.31.0-1.1
+# upgrade the K8s cluster
+kubeadm upgrade plan v1.31.0
+kubeadm upgrade apply v1.31.0
+# upgrade the kubelet, then mark the cp node as schedulable
+apt-get install kubelet=1.31.0-1.1
+kubectl uncordon cluster2-controlplane
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"># TODO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>check since which command was this node made un-schdeulable
+systemctl daemon-reload
+systemctl restart kubelet</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># enable file_output in /etc/falco/falco.yaml
+file_output:
+  enabled: true
+  keep_alive: false
+  filename: /opt/security_incidents/alerts.log  # where you will log the alerts
+# add the update rule under the /etc/falco/falco_rules.local.yaml
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t># TODO:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">do you copy this from falco.yaml and just change the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>output:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>priority</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>?
+- rule: Write below binary dir
+  desc: an attempt to write to any file below a set of binary directories
+  condition: &gt;
+    bin_dir and evt.dir = &lt; and open_write
+    and not package_mgmt_procs
+    and not exe_running_docker_save
+    and not python_running_get_pip
+    and not python_running_ms_oms
+    and not user_known_write_below_binary_dir_activities
+  output: &gt;
+    File below a known binary directory opened for writing (user_id=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>%user.uid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> file_updated=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>%fd.name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> command=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>%proc.cmdline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">)
+  priority: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>CRITICAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+  tags: [filesystem, mitre_persistence]
+# hot reload: only update necesary part, keep existing session/connection, suitable for HA, config/partial code update
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>kill -1 $(cat /var/run/falco.pid)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+# or restart the service: clean up old states, all services supported, impact on high traffic services
+systemctl restart falco</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vi Dockerfile
+FROM alpine:3.12                              # change this
+RUN apk update &amp;&amp; apk add vim nginx&gt;=1.18.0   # change this
+RUN addgroup -S myuser &amp;&amp; adduser -S myuser -G myuser
+COPY ./run.sh run.sh
+RUN ["chmod", "+x", "./run.sh"]
+USER newuser                                  # change this
+ENTRYPOINT ["/bin/sh" , "./run.sh"]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"># TODO: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>what about the no-curl part?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>securityContext
+runAsUser
+capabilities.add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k get po ubuntu-sleeper -oyaml &gt; 3-5.yaml
+vi 3-5.yaml
+…
+spec:
+  containers:
+  - image: ubuntu
+    securityContext:
+      runAsUser: 0
+      capabilities:
+        add: ["SYS_TIME"]
+…
+k replace --force -f 3-5.yaml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ImagePolicyWebhook
+AdmissionController
+AdmissionConfiguration
+admission-control-config-file
+enable-admission-plugins
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vi /etc/kubernetes/pki/admission_configuration.yaml
+# To set the policy to implicit deny
+...
+plugins:
+- name: ImagePolicyWebhook
+  configuration:
+    imagePolicy:
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>defaultAllow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">: false 
+# To add the kubeconfig file already created ImagePolicyWebhook resources
+...
+plugins:
+- name: ImagePolicyWebhook
+  configuration:
+    imagePolicy:
+      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>kubeConfigFile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>: /etc/kubernetes/pki/admission_kube_config.yaml
+vi /etc/kubernetes/manifests/kube-apiserver.yaml
+    - --enable-admission-plugins=NodeRestriction,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>ImagePolicyWebhook</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> - --admission-control-config-file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>=/etc/kubernetes/pki/admission_configuration.yaml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Immutable pods
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># if `readOnlyRootFilesystem` exists and is set to true, then it's good and shouldn't be deleted.
+# if `privileged` exists and is set to true, then we need to delete this pod definition file.
+# if `readOnlyRootFilesytem` is not defined, we should delete that pod definition file as well.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sevice type
+unexposing ports to minimize external access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k -n system-hardening get svc nginx-external-service -oyaml &gt; 3-8.yaml
+vi 3-8.yaml
+apiVersion: v1
+kind: Service
+metadata:
+  name: nginx-external-service
+  namespace: system-hardening
+spec:
+  selector:
+    app: nginx-external
+  ports:
+    - name: http
+      protocol: TCP
+      port: 80
+      targetPort: 80
+    - name: https
+      protocol: TCP
+      port: 443
+      targetPort: 443
+  type: ClusterIP       # change this and remove nodeport number
+# esc and save
+k replace --force -f 3-8.yaml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -625,6 +1850,38 @@
       <color theme="1"/>
       <name val="Menlo Regular"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Menlo Regular"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -672,7 +1929,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -705,6 +1962,27 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1022,36 +2300,422 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88647C6-48F9-7245-B94A-FFCF930897A6}">
   <sheetPr>
-    <tabColor rgb="FF7030A0"/>
+    <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="6" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="145.1640625" style="11" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>123</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="208">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="256">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="96">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
+        <v>3</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="144">
+      <c r="A8" s="13">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48">
+      <c r="A9" s="13">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13">
+        <v>5</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="409.6">
+      <c r="A10" s="13">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="160">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13">
+        <v>7</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="365">
+      <c r="A12" s="13">
+        <v>1</v>
+      </c>
+      <c r="B12" s="13">
+        <v>8</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="409" customHeight="1">
+      <c r="A13" s="13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="320">
+      <c r="A14" s="13">
+        <v>2</v>
+      </c>
+      <c r="B14" s="13">
+        <v>2</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="48">
+      <c r="A15" s="13">
+        <v>2</v>
+      </c>
+      <c r="B15" s="13">
+        <v>3</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="272">
+      <c r="A16" s="13">
+        <v>2</v>
+      </c>
+      <c r="B16" s="13">
+        <v>4</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="160">
+      <c r="A17" s="13">
+        <v>2</v>
+      </c>
+      <c r="B17" s="13">
+        <v>5</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="128">
+      <c r="A18" s="13">
+        <v>2</v>
+      </c>
+      <c r="B18" s="13">
+        <v>6</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="144">
+      <c r="A19" s="13">
+        <v>2</v>
+      </c>
+      <c r="B19" s="13">
+        <v>7</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="48">
+      <c r="A20" s="13">
+        <v>2</v>
+      </c>
+      <c r="B20" s="13">
+        <v>8</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="408" customHeight="1">
+      <c r="A21" s="16">
+        <v>2</v>
+      </c>
+      <c r="B21" s="16">
+        <v>9</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="140" customHeight="1">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="1:4" ht="80">
+      <c r="A23" s="13">
+        <v>3</v>
+      </c>
+      <c r="B23" s="13">
+        <v>1</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="64">
+      <c r="A24" s="13">
+        <v>3</v>
+      </c>
+      <c r="B24" s="13">
+        <v>2</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="48">
+      <c r="A25" s="13">
+        <v>3</v>
+      </c>
+      <c r="B25" s="13">
+        <v>3</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="365">
+      <c r="A26" s="13">
+        <v>3</v>
+      </c>
+      <c r="B26" s="13">
+        <v>4</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="204">
+      <c r="A27" s="13">
+        <v>3</v>
+      </c>
+      <c r="B27" s="13">
+        <v>5</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="320">
+      <c r="A28" s="13">
+        <v>3</v>
+      </c>
+      <c r="B28" s="13">
+        <v>6</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="48">
+      <c r="A29" s="13">
+        <v>3</v>
+      </c>
+      <c r="B29" s="13">
+        <v>7</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="350">
+      <c r="A30" s="13">
+        <v>3</v>
+      </c>
+      <c r="B30" s="13">
+        <v>8</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{0D28C639-3FFD-F64A-8D8A-298EE36BB2C9}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{B19453C2-609D-434D-9292-A2C123B814C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1123,8 +2787,8 @@
   </sheetPr>
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="141" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A11" zoomScale="141" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1757,7 +3421,7 @@
   </sheetPr>
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
@@ -2225,7 +3889,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
complete killer rehearsal; killercoda 22 scenarios left
</commit_message>
<xml_diff>
--- a/cks_kcsa_kcna.xlsx
+++ b/cks_kcsa_kcna.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiwen/Documents/wysi/project-cyber-monday/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7F4E49-9B51-AC41-A566-89C96781690A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729DB672-5DE6-C24F-884B-1228D70DDC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18600" yWindow="-1460" windowWidth="18600" windowHeight="20020" xr2:uid="{87DCA1D7-EB5D-4C4C-A7D2-7199B399E110}"/>
+    <workbookView xWindow="-24900" yWindow="1180" windowWidth="23860" windowHeight="17800" activeTab="4" xr2:uid="{87DCA1D7-EB5D-4C4C-A7D2-7199B399E110}"/>
   </bookViews>
   <sheets>
     <sheet name="kk_CKS" sheetId="3" r:id="rId1"/>
     <sheet name="kk_KCNA" sheetId="4" state="hidden" r:id="rId2"/>
     <sheet name="kk_KCSA" sheetId="5" state="hidden" r:id="rId3"/>
-    <sheet name="killercoda_CKS" sheetId="8" r:id="rId4"/>
-    <sheet name="killer.sh_CKS" sheetId="9" r:id="rId5"/>
+    <sheet name="killer.sh_CKS" sheetId="9" r:id="rId4"/>
+    <sheet name="killercoda_CKS" sheetId="8" r:id="rId5"/>
     <sheet name="pluralsight_KCNA" sheetId="6" state="hidden" r:id="rId6"/>
     <sheet name="freecodecamp_KCNA" sheetId="7" state="hidden" r:id="rId7"/>
     <sheet name="other_resources" sheetId="10" r:id="rId8"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="199">
   <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1789,12 +1789,850 @@
     <t>Attempt-5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Nope.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># allows all Pods in Namespace app to only connect to Pods with labels id: data in Namespace data
+apiVersion: "cilium.io/v2"
+kind: CiliumNetworkPolicy
+metadata:
+  name: policy1
+  namespace: app
+spec:
+  endpointSelector:
+    matchLabels: {}
+  egress:
+  - toEndpoints:
+    - matchLabels:
+        io.kubernetes.pod.namespace: data
+        id: data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi ~/.vimrc
+set expandtab
+set tabstop=2
+set shiftwidth=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cat /var/log/syslog | grep apiserver
+cd /var/log/pods/kube-system_kube-apiserver-controlplane_XXX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ssh node01
+cat /etc/kubernetes/kubelet.conf 
+export KUBECONFIG=/etc/kubernetes/kubelet.conf
+k label node controlplane killercoda/one=123
+k label node node01 node-restriction.kubernetes.io/one=123
+vi /etc/kubernetes/manifests/kube-apiserver.yaml 
+spec:
+  containers:
+  - command:
+    ... 
+    - --enable-admission-plugins=NodeRestriction
+ssh node01
+export KUBECONFIG=/etc/kubernetes/kubelet.conf
+k label node controlplane killercoda/two=123
+k label node node01 node-restriction.kubernetes.io/two=123
+k label node node01 test/two=123 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># kill an unwanted process listening on port 1234
+apt install net-tools
+netstat -tulpan | grep 1234
+lsof -i :1234
+# find pull path
+ls -l /proc/14390/exe
+kill 14390
+# delete the pull path/binary
+rm /usr/bin/app1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>cat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> /var/log/pods/kube-system_kube-apiserver-controlplane</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>_36b3bac598f6bd76f4b97286d2bcb99b/kube-apiserver/X.log 
+2024-12-31T06:22:08.80934717Z stderr F Error: unknown flag: --this-is-very-wrong
+# check pod log
+cd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> /var/log/pods/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">kube-system_kube-apiserver-controlplane_XXX
+crictl ps
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>crictl logs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> 497ad50c47b4d    # containerID of kube-apiserver
+# check syslog
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>journalctl | grep apiserver</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+cat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> /var/log/syslog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> | grep apiserver 
+tail -f /var/log/syslog | grep apiserver</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># remove kube-bench of package manager
+apt show kube-bench
+apt remove kube-bench
+# stop the vsftpd service
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>lsof -i :21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+service vsftpd stop
+lsof -I :21</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>sha512sum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> /usr/bin/kubelet
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>sha512sum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> kubernetes/server/bin/kubelet</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># strace will list various syscalls a process makes
+strace kill -9 1234
+strace kill -9 1234 2&gt;&amp;1 | grep 1234
+strace kill -15 1234
+strace kill -15 1234 2&gt;&amp;1 | grep 1234
+strace nc -l -p 8080 2&gt;&amp;1 | grep 8080
+ps aux | grep kube-apiserver
+strace -p &lt;pid-of-kube-apiserver&gt; -f
+strace -p 2219 -f -cw
+strace: Process 2219 attached with 7 threads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>When it comes to manual analysis of K8s manifest files, use below checks:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+securityContext:
+  readOnlyRootFilesystem: true
+  allowPrivilegeEscalation: false
+  privileged: false</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FROM ubuntu  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t># larger for building</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+ARG DEBIAN_FRONTEND=noninteractive
+RUN apt-get update &amp;&amp; apt-get install -y golang-go
+COPY app.go .
+RUN CGO_ENABLED=0 go build app.go
+FROM alpine.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> # smaller for running - multiple stages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+COPY --from=0 /app .
+CMD ["./app"]
+---
+...
+COPY --from=0 /app /home/appuser/
+USER appuser </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> # not running a containerised application as root</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+CMD ["/home/appuser/app"]
+---
+FROM ubuntu
+...
+RUN echo $SECRET_TOKEN &gt; /tmp/token </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t># still persist as layer in the container</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+RUN /etc/register.sh /tmp/token
+RUN rm /tmp/token</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> # although being deleted later</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+EXPOSE 3306
+CMD ["/run.sh"]</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># pod-definition.yaml
+spec:
+  automountServiceAccountToken: false
+# apply &amp; verify
+kubectl -n one exec -it pod-one -- mount | grep serviceaccount
+kubectl -n one exec -it pod-one -- cat /var/run/secrets/kubernetes.io/serviceaccount/token
+# sa-definition.yaml
+apiVersion: v1
+kind: ServiceAccount
+automountServiceAccountToken: false
+# edit &amp; verify
+kubectl -n two exec -it pod-two -- mount | grep serviceaccount
+kubectl -n two exec -it pod-two -- cat /var/run/secrets/kubernetes.io/serviceaccount/token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># from-literal
+k -n ns-secure create secret generic sec-a1 --from-literal user=admin
+# from-file
+k -n ns-secure create secret generic sec-a2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>--from-file index=/etc/hosts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+k -n ns-secure run secret-manager --image httpd:alpine --dry-run=client -oyaml &gt; 34-2.yaml
+vi 34-2.yaml
+...
+spec:
+  volumes:                            # mount as volume
+  - name: sec-a2                      # add
+    secret:                           # add
+      secretName: sec-a2              # add
+  serviceAccountName: secret-manager  # add 
+  containers:
+  - name: secret-manager
+    volumeMounts:             # mount as volume, readonly
+    - name: sec-a2            # add
+      mountPath: /etc/sec-a2  # add
+      readOnly: true          # add
+    env:                
+    - name: SEC_A1      # add as environment variable
+      valueFrom:        # add
+        secretKeyRef:   # add
+          name: sec-a1  # add
+          key: user     # add</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">k get secret -n one
+NAME   TYPE     DATA   AGE
+s1     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>Opaque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">   1      93s
+s2     Opaque   1      93s
+echo $(kubectl -n one get secret s1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>-ojsonpath="{.data.data}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> | base64 -d) &gt;&gt; /opt/ks/one
+echo $(kubectl -n one get secret s2 -ojsonpath="{.data.data}" | base64 -d) &gt;&gt; /opt/ks/one
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">k -n applications create role smoke --verb create,delete --resource pods,deployments,sts
+k -n applications create </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>rolebinding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> smoke --</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>role</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> smoke --user smoke
+k get ns
+k -n applications create </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>rolebinding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> smoke-view --</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>clusterrole</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> view --user smoke
+k -n default create </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>rolebinding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> smoke-view --</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>clusterrole</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> view --user smoke
+k -n kube-node-lease create </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>rolebinding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> smoke-view --</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>clusterrole</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> view --user smoke
+k -n kube-public create </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>rolebinding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> smoke-view --</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>clusterrole</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> view --user smoke
+# Just list secret names, no content.   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>BEAWARE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> list secret role also allows user to see credentials (possible mis-configuration!)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># create runtime class
+apiVersion: node.k8s.io/v1
+kind: RuntimeClass
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">metadata:
+  name: gvisor
+handler: runsc
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"># create pod
+apiVersion: v1
+kind: Pod
+metadata:
+  name: sec
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">spec:
+  runtimeClassName: gvisor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">  containers:
+    - image: nginx:1.21.5-alpine
+      name: sec
+# verify runtime of the pod/sec by dmesg tool
+k exec sec -- dmesg | grep -i gvisor</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># create encryptionconfiguration
+mkdir -p /etc/kubernetes/etcd
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>echo -n this-is-very-sec | base64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+cat &lt;&lt;EOF&gt; /etc/kubernetes/etcd/ec.yaml
+apiVersion: apiserver.config.k8s.io/v1
+kind: EncryptionConfiguration
+resources:
+  - resources:
+    - secrets
+    providers:
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">- aesgcm:  # provider type: asegcm
+        keys:
+        - name: key1
+          secret: dGhpcy1pcy12ZXJ5LXNlYw==
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">          # all new secrets should be encrypted with this
+    - identity: {} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t># the other provider: can read existing unencrypted secrets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve">
+EOF
+# at apiserver config yaml file, add args:
+- command:
+  - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>--encryption-provider-config</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>=/etc/kubernetes/etcd/ec.yaml
+# at apiserver config yaml file, add volume:
+    volumes:
+    - hostPath:
+      path: /etc/kubernetes/etcd
+      type: DirectoryOrCreate
+    name: etcd
+# at apiserver config yaml file, add volumeMounts:
+    volumeMounts:
+    - mountPath: /etc/kubernetes/etcd
+      name: etcd
+      readOnly: true</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1813,12 +2651,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1844,11 +2676,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Menlo Regular"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1893,6 +2720,37 @@
       <color theme="0"/>
       <name val="Menlo Regular"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2F3337"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Menlo Regular"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1908,7 +2766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1931,75 +2789,122 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2321,7 +3226,7 @@
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -2329,255 +3234,255 @@
   <cols>
     <col min="1" max="2" width="6" style="1" customWidth="1"/>
     <col min="3" max="3" width="39.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="145.1640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="145.1640625" style="5" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="7" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="208">
-      <c r="A5" s="11">
+      <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="8" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="256">
-      <c r="A6" s="11">
+      <c r="A6" s="7">
         <v>1</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="7">
         <v>2</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="8" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="80">
-      <c r="A7" s="11">
+      <c r="A7" s="7">
         <v>1</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="144">
-      <c r="A8" s="11">
+      <c r="A8" s="7">
         <v>1</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="8" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="48">
-      <c r="A9" s="11">
+      <c r="A9" s="7">
         <v>1</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="8" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="409.6">
-      <c r="A10" s="11">
+      <c r="A10" s="7">
         <v>1</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="7">
         <v>6</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="160">
-      <c r="A11" s="11">
+      <c r="A11" s="7">
         <v>1</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="7">
         <v>7</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="365">
-      <c r="A12" s="11">
+      <c r="A12" s="7">
         <v>1</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="7">
         <v>8</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="8" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="409" customHeight="1">
-      <c r="A13" s="11">
+      <c r="A13" s="7">
         <v>2</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="7">
         <v>1</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="8" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="320">
-      <c r="A14" s="11">
+      <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="7">
         <v>2</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="8" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48">
-      <c r="A15" s="11">
+      <c r="A15" s="7">
         <v>2</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="7">
         <v>3</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="8" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="272">
-      <c r="A16" s="11">
+      <c r="A16" s="7">
         <v>2</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="7">
         <v>4</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="8" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="160">
-      <c r="A17" s="11">
+      <c r="A17" s="7">
         <v>2</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="7">
         <v>5</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="8" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="128">
-      <c r="A18" s="11">
+      <c r="A18" s="7">
         <v>2</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="7">
         <v>6</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="8" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="144">
-      <c r="A19" s="11">
+      <c r="A19" s="7">
         <v>2</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="7">
         <v>7</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="8" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="48">
-      <c r="A20" s="11">
+      <c r="A20" s="7">
         <v>2</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="7">
         <v>8</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="8" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2602,122 +3507,122 @@
       <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" ht="80">
-      <c r="A23" s="11">
+      <c r="A23" s="7">
         <v>3</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="7">
         <v>1</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="8" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="64">
-      <c r="A24" s="11">
+      <c r="A24" s="7">
         <v>3</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="7">
         <v>2</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="7" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="48">
-      <c r="A25" s="11">
+      <c r="A25" s="7">
         <v>3</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="7">
         <v>3</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="365">
-      <c r="A26" s="11">
+      <c r="A26" s="7">
         <v>3</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="7">
         <v>4</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="8" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="204">
-      <c r="A27" s="11">
+      <c r="A27" s="7">
         <v>3</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="7">
         <v>5</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="6" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="320">
-      <c r="A28" s="11">
+      <c r="A28" s="7">
         <v>3</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="7">
         <v>6</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="8" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="48">
-      <c r="A29" s="11">
+      <c r="A29" s="7">
         <v>3</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29" s="7">
         <v>7</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="8" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="350">
-      <c r="A30" s="11">
+      <c r="A30" s="7">
         <v>3</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30" s="7">
         <v>8</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="8" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2753,7 +3658,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2784,7 +3689,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2798,640 +3703,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D1593A-60CA-7447-B941-D38AFCB595A5}">
-  <sheetPr>
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
-  <dimension ref="A1:G44"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="3.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.1640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="3">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="3">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="3">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="3">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="196">
-      <c r="B10" s="3">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" s="3">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="3">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="3">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="3">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="3">
-        <v>12</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="3">
-        <v>13</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="3">
-        <v>14</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="3">
-        <v>15</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="3">
-        <v>16</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="3">
-        <v>17</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="3">
-        <v>18</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="3">
-        <v>19</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="3">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="3">
-        <v>21</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="3">
-        <v>22</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="3">
-        <v>23</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="3">
-        <v>24</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="3">
-        <v>25</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="3">
-        <v>26</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="3">
-        <v>27</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="3">
-        <v>28</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="B32" s="3">
-        <v>29</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="2:7">
-      <c r="B33" s="3">
-        <v>30</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="3">
-        <v>31</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="2:7">
-      <c r="B35" s="3">
-        <v>32</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="2:7">
-      <c r="B36" s="3">
-        <v>33</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="2:7">
-      <c r="B37" s="3">
-        <v>34</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="2:7">
-      <c r="B38" s="3">
-        <v>35</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="2:7">
-      <c r="B39" s="3">
-        <v>36</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="2:7">
-      <c r="B40" s="3">
-        <v>37</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="2:7">
-      <c r="B41" s="3">
-        <v>38</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="2:7">
-      <c r="B42" s="3">
-        <v>39</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="2:7">
-      <c r="B43" s="3">
-        <v>40</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="2:7">
-      <c r="B44" s="3">
-        <v>41</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="Link to killercoda at Youtube" xr:uid="{801F38EF-1198-7149-A133-DDF4B4E36FBD}"/>
-    <hyperlink ref="F10" r:id="rId2" xr:uid="{1B375D11-4F36-F646-838B-AFBFC10B7FF9}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787FC8CE-F471-4541-8EC6-C6DDD4D0E6CF}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
@@ -3439,14 +3710,14 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" style="1" customWidth="1"/>
     <col min="5" max="9" width="15.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
@@ -3455,972 +3726,972 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="9"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5">
         <v>3</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5">
         <v>3</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5">
         <v>3</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5">
         <v>4</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5">
         <v>4</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5">
         <v>4</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5">
         <v>5</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5">
         <v>5</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5">
         <v>5</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5">
         <v>6</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5">
         <v>6</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5">
         <v>6</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5">
         <v>7</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5">
         <v>7</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5">
         <v>7</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5">
         <v>8</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5">
         <v>8</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5">
         <v>8</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5">
         <v>9</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5">
         <v>9</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5">
         <v>9</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5">
         <v>10</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5">
         <v>10</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5">
         <v>10</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5">
         <v>11</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5">
         <v>11</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5">
         <v>11</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5">
         <v>12</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5">
         <v>12</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5">
         <v>12</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5">
         <v>13</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5">
         <v>13</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5">
         <v>13</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5">
         <v>14</v>
       </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5">
         <v>14</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5">
         <v>14</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5">
         <v>15</v>
       </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5">
         <v>15</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5">
         <v>15</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5">
         <v>16</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5">
         <v>16</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5">
         <v>16</v>
       </c>
-      <c r="C49" s="17"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5">
         <v>17</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5">
         <v>17</v>
       </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5">
         <v>17</v>
       </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="9"/>
-      <c r="B53" s="9">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5">
         <v>18</v>
       </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5">
         <v>18</v>
       </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5">
         <v>18</v>
       </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5">
         <v>19</v>
       </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5">
         <v>19</v>
       </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5">
         <v>19</v>
       </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="9"/>
-      <c r="B59" s="9">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5">
         <v>20</v>
       </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5">
         <v>20</v>
       </c>
-      <c r="C60" s="17"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5">
         <v>20</v>
       </c>
-      <c r="C61" s="17"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5">
         <v>21</v>
       </c>
-      <c r="C62" s="17"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="9"/>
-      <c r="B63" s="9">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5">
         <v>21</v>
       </c>
-      <c r="C63" s="17"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5">
         <v>21</v>
       </c>
-      <c r="C64" s="17"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
-      <c r="J64" s="9"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="9"/>
-      <c r="B65" s="9">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5">
         <v>22</v>
       </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-      <c r="J65" s="9"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5">
         <v>22</v>
       </c>
-      <c r="C66" s="17"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5">
         <v>22</v>
       </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4429,6 +4700,690 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D1593A-60CA-7447-B941-D38AFCB595A5}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:G45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D36" sqref="D34:D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="110.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="109.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="18">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" ht="240">
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" ht="64">
+      <c r="B6" s="18">
+        <v>3</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" ht="240">
+      <c r="B7" s="18">
+        <v>4</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" ht="48">
+      <c r="B8" s="18">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" ht="320">
+      <c r="B9" s="18">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" ht="224">
+      <c r="B10" s="18">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="18">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="18">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="18">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="18">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="18">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="18">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="18">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="18">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="18">
+        <v>16</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="18">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="18">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="18">
+        <v>19</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="18">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="18">
+        <v>21</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="18">
+        <v>22</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="18">
+        <v>23</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="18">
+        <v>24</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="18">
+        <v>25</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="18">
+        <v>26</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="18">
+        <v>27</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="18">
+        <v>28</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" ht="170">
+      <c r="B32" s="18">
+        <v>29</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7" ht="288">
+      <c r="B33" s="18">
+        <v>30</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" ht="409.6" customHeight="1">
+      <c r="B34" s="25">
+        <v>31</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="2:7" ht="74" customHeight="1">
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="18">
+        <v>32</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="2:7" ht="112">
+      <c r="B37" s="18">
+        <v>33</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" ht="409.6">
+      <c r="B38" s="18">
+        <v>34</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+    </row>
+    <row r="39" spans="2:7" ht="256">
+      <c r="B39" s="18">
+        <v>35</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+    </row>
+    <row r="40" spans="2:7" ht="372">
+      <c r="B40" s="18">
+        <v>36</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+    </row>
+    <row r="41" spans="2:7" ht="96">
+      <c r="B41" s="18">
+        <v>37</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+    </row>
+    <row r="42" spans="2:7" ht="208">
+      <c r="B42" s="18">
+        <v>38</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+    </row>
+    <row r="43" spans="2:7" ht="160">
+      <c r="B43" s="18">
+        <v>39</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+    </row>
+    <row r="44" spans="2:7" ht="112">
+      <c r="B44" s="18">
+        <v>40</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+    </row>
+    <row r="45" spans="2:7" ht="32">
+      <c r="B45" s="18">
+        <v>41</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B34:B35"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="Link to killercoda at Youtube" xr:uid="{801F38EF-1198-7149-A133-DDF4B4E36FBD}"/>
+    <hyperlink ref="F10" r:id="rId2" xr:uid="{1B375D11-4F36-F646-838B-AFBFC10B7FF9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4446,7 +5401,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1" ht="16">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4476,7 +5431,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4503,7 +5458,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="1"/>
@@ -4581,7 +5536,7 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1"/>
@@ -4619,7 +5574,7 @@
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="1"/>

</xml_diff>